<commit_message>
minor changes in model
</commit_message>
<xml_diff>
--- a/model/data/genesys-mod.xlsx
+++ b/model/data/genesys-mod.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwickl-nb\Desktop\downscaling-optimization\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zwickl-nb\GitHub\Downscaling-paper-manuscript\model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="22">
   <si>
     <t>model</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>2050</t>
-  </si>
-  <si>
-    <t>2051</t>
   </si>
 </sst>
 </file>
@@ -102,7 +99,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,17 +126,6 @@
       <color theme="1"/>
       <name val="Segoe UI Light"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Segoe UI Light"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Segoe UI Light"/>
     </font>
   </fonts>
   <fills count="3">
@@ -169,68 +155,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <b val="0"/>
@@ -392,6 +329,29 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -406,24 +366,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:G37" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2">
-  <autoFilter ref="A1:G37">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Directed Transition"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <tableColumns count="7">
-    <tableColumn id="1" name="model" dataDxfId="8"/>
-    <tableColumn id="2" name="scenario" dataDxfId="7"/>
-    <tableColumn id="3" name="region" dataDxfId="6"/>
-    <tableColumn id="4" name="variable" dataDxfId="5"/>
-    <tableColumn id="5" name="unit" dataDxfId="4"/>
-    <tableColumn id="6" name="2050" dataDxfId="3" dataCellStyle="Komma"/>
-    <tableColumn id="7" name="2051" dataDxfId="0">
-      <calculatedColumnFormula>Tabelle1[[#This Row],[2050]]/3.6</calculatedColumnFormula>
-    </tableColumn>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:F37" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F37"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="model" dataDxfId="5"/>
+    <tableColumn id="2" name="scenario" dataDxfId="4"/>
+    <tableColumn id="3" name="region" dataDxfId="3"/>
+    <tableColumn id="4" name="variable" dataDxfId="2"/>
+    <tableColumn id="5" name="unit" dataDxfId="1"/>
+    <tableColumn id="6" name="2050" dataDxfId="0" dataCellStyle="Komma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -692,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
@@ -707,7 +658,7 @@
     <col min="5" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -726,11 +677,8 @@
       <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -750,12 +698,8 @@
         <f>19.336003086675-7.2</f>
         <v>12.136003086675</v>
       </c>
-      <c r="G2" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>3.3711119685208333</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -774,12 +718,8 @@
       <c r="F3" s="4">
         <v>7.6532547687941284</v>
       </c>
-      <c r="G3" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>2.1259041024428136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -798,12 +738,8 @@
       <c r="F4" s="4">
         <v>81.811449191463808</v>
       </c>
-      <c r="G4" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>22.725402553184392</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -823,12 +759,8 @@
         <f>70.1906681163622-7.2</f>
         <v>62.990668116362201</v>
       </c>
-      <c r="G5" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>17.497407810100611</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -847,12 +779,8 @@
       <c r="F6" s="5">
         <v>3.7069700000000001</v>
       </c>
-      <c r="G6" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>1.0297138888888888</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -872,12 +800,8 @@
         <f>3.6*2</f>
         <v>7.2</v>
       </c>
-      <c r="G7" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -897,12 +821,8 @@
         <f>2*3.6</f>
         <v>7.2</v>
       </c>
-      <c r="G8" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -921,12 +841,8 @@
       <c r="F9" s="2">
         <v>1.28</v>
       </c>
-      <c r="G9" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>0.35555555555555557</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -946,12 +862,8 @@
         <f>12.14</f>
         <v>12.14</v>
       </c>
-      <c r="G10" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>3.3722222222222222</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -970,12 +882,8 @@
       <c r="F11" s="4">
         <v>6.5024817912461899</v>
       </c>
-      <c r="G11" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>1.8062449420128304</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
@@ -994,12 +902,8 @@
       <c r="F12" s="4">
         <v>31.153744</v>
       </c>
-      <c r="G12" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>8.6538177777777783</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -1018,12 +922,8 @@
       <c r="F13" s="4">
         <v>34.839105097971164</v>
       </c>
-      <c r="G13" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>9.6775291938808792</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
@@ -1043,12 +943,8 @@
         <f>76.3702188624354-7.2</f>
         <v>69.170218862435391</v>
       </c>
-      <c r="G14" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>19.21394968400983</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
@@ -1067,12 +963,8 @@
       <c r="F15" s="4">
         <v>0</v>
       </c>
-      <c r="G15" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
@@ -1092,12 +984,8 @@
         <f>2*3.6</f>
         <v>7.2</v>
       </c>
-      <c r="G16" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
@@ -1117,12 +1005,8 @@
         <f>3.6*2</f>
         <v>7.2</v>
       </c>
-      <c r="G17" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
@@ -1141,12 +1025,8 @@
       <c r="F18" s="2">
         <v>19.255230000000001</v>
       </c>
-      <c r="G18" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>5.3486750000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>8</v>
       </c>
@@ -1166,12 +1046,8 @@
         <f>12.14</f>
         <v>12.14</v>
       </c>
-      <c r="G19" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>3.3722222222222222</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>8</v>
       </c>
@@ -1190,12 +1066,8 @@
       <c r="F20" s="4">
         <v>7.1129852895145183</v>
       </c>
-      <c r="G20" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>1.9758292470873662</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -1214,12 +1086,8 @@
       <c r="F21" s="5">
         <v>7.83833</v>
       </c>
-      <c r="G21" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>2.177313888888889</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>8</v>
       </c>
@@ -1239,12 +1107,8 @@
         <f>77.2976103400594-7.2</f>
         <v>70.097610340059404</v>
       </c>
-      <c r="G22" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>19.471558427794278</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>8</v>
       </c>
@@ -1263,12 +1127,8 @@
       <c r="F23" s="4">
         <v>56.568454824038355</v>
       </c>
-      <c r="G23" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>15.713459673343987</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>8</v>
       </c>
@@ -1287,12 +1147,8 @@
       <c r="F24" s="4">
         <v>7.2</v>
       </c>
-      <c r="G24" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>8</v>
       </c>
@@ -1311,12 +1167,8 @@
       <c r="F25" s="4">
         <v>7.2</v>
       </c>
-      <c r="G25" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>8</v>
       </c>
@@ -1335,12 +1187,8 @@
       <c r="F26" s="4">
         <v>4.8468</v>
       </c>
-      <c r="G26" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>1.3463333333333334</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
         <v>8</v>
       </c>
@@ -1360,12 +1208,8 @@
         <f>19.336003086675-7.2</f>
         <v>12.136003086675</v>
       </c>
-      <c r="G27" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>3.3711119685208333</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
         <v>8</v>
       </c>
@@ -1384,12 +1228,8 @@
       <c r="F28" s="4">
         <v>7.2</v>
       </c>
-      <c r="G28" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
         <v>8</v>
       </c>
@@ -1408,12 +1248,8 @@
       <c r="F29" s="4">
         <v>5.5246594240112818</v>
       </c>
-      <c r="G29" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>1.5346276177809115</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>8</v>
       </c>
@@ -1432,12 +1268,8 @@
       <c r="F30" s="4">
         <v>26.741028</v>
       </c>
-      <c r="G30" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>7.4280633333333332</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
         <v>8</v>
       </c>
@@ -1456,12 +1288,8 @@
       <c r="F31" s="4">
         <v>93.473087609196369</v>
       </c>
-      <c r="G31" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>25.9647465581101</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>8</v>
       </c>
@@ -1481,12 +1309,8 @@
         <f>24.0984325061292-7.2</f>
         <v>16.8984325061292</v>
       </c>
-      <c r="G32" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>4.6940090294803332</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
         <v>8</v>
       </c>
@@ -1505,12 +1329,8 @@
       <c r="F33" s="4">
         <v>7.2</v>
       </c>
-      <c r="G33" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
         <v>8</v>
       </c>
@@ -1529,12 +1349,8 @@
       <c r="F34" s="4">
         <v>0</v>
       </c>
-      <c r="G34" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>8</v>
       </c>
@@ -1553,12 +1369,8 @@
       <c r="F35" s="4">
         <v>0</v>
       </c>
-      <c r="G35" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
         <v>8</v>
       </c>
@@ -1577,12 +1389,8 @@
       <c r="F36" s="4">
         <v>0</v>
       </c>
-      <c r="G36" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>8</v>
       </c>
@@ -1600,10 +1408,6 @@
       </c>
       <c r="F37" s="4">
         <v>10.037000000000001</v>
-      </c>
-      <c r="G37" s="6">
-        <f>Tabelle1[[#This Row],[2050]]/3.6</f>
-        <v>2.7880555555555557</v>
       </c>
     </row>
   </sheetData>

</xml_diff>